<commit_message>
improve reproduction of figure 5
</commit_message>
<xml_diff>
--- a/src/surmeier_lab_to_nwb/zhai2025/assets/author_assets/Key resources table_Zhai_v1.xlsx
+++ b/src/surmeier_lab_to_nwb/zhai2025/assets/author_assets/Key resources table_Zhai_v1.xlsx
@@ -751,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -799,6 +799,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1118,26 +1121,26 @@
     <col min="4" max="4" style="17" width="54.71928571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="18" width="11.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1984,7 +1987,7 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18">
       <c r="A23" s="7" t="s">
         <v>66</v>
       </c>
@@ -2064,7 +2067,7 @@
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
       <c r="A25" s="7" t="s">
         <v>75</v>
       </c>
@@ -2102,7 +2105,7 @@
       <c r="Y25" s="7"/>
       <c r="Z25" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
       <c r="A26" s="3" t="s">
         <v>75</v>
       </c>

</xml_diff>